<commit_message>
FeatureRM #381 (mux_squid): Add debug variant tests (*.json) and create 2 test name in order to:   . loop on all debug variant tests   . loop on all functional variant tests.
</commit_message>
<xml_diff>
--- a/simu/conf/fpasim/mux_squid/mux_squid_top_test_list.xlsx
+++ b/simu/conf/fpasim/mux_squid/mux_squid_top_test_list.xlsx
@@ -31,6 +31,9 @@
       <style:table-column-properties fo:break-before="auto" style:column-width="6.371cm"/>
     </style:style>
     <style:style style:name="co4" style:family="table-column">
+      <style:table-column-properties fo:break-before="auto" style:column-width="9.095cm"/>
+    </style:style>
+    <style:style style:name="co5" style:family="table-column">
       <style:table-column-properties fo:break-before="auto" style:column-width="2.258cm"/>
     </style:style>
     <style:style style:name="ro1" style:family="table-row">
@@ -42,11 +45,15 @@
     <style:style style:name="ro3" style:family="table-row">
       <style:table-row-properties style:row-height="0.788cm" fo:break-before="auto" style:use-optimal-row-height="false"/>
     </style:style>
+    <style:style style:name="ro4" style:family="table-row">
+      <style:table-row-properties style:row-height="4.396cm" fo:break-before="auto" style:use-optimal-row-height="true"/>
+    </style:style>
     <style:style style:name="ta1" style:family="table" style:master-page-name="Default">
       <style:table-properties table:display="true" style:writing-mode="lr-tb"/>
     </style:style>
-    <style:style style:name="ce1" style:family="table-cell" style:parent-style-name="Default">
-      <style:table-cell-properties fo:background-color="#00a933"/>
+    <style:style style:name="ce5" style:family="table-cell" style:parent-style-name="Default">
+      <style:table-cell-properties fo:background-color="#00a933" style:text-align-source="fix" style:repeat-content="false" style:vertical-align="middle"/>
+      <style:paragraph-properties fo:text-align="center" fo:margin-left="0cm"/>
     </style:style>
     <style:style style:name="ce2" style:family="table-cell" style:parent-style-name="Default">
       <style:table-cell-properties style:text-align-source="fix" style:repeat-content="false" style:vertical-align="middle"/>
@@ -71,6 +78,12 @@
     </style:style>
     <style:style style:name="T1" style:family="text">
       <style:text-properties style:font-name="Liberation Sans" fo:font-size="10pt" fo:font-weight="normal" style:text-underline-style="none" style:text-underline-color="font-color" style:text-line-through-type="none" fo:font-style="normal" style:text-outline="false" fo:text-shadow="none" style:text-line-through-mode="continuous" fo:language="fr" fo:country="FR" style:language-asian="zh" style:country-asian="CN" style:language-complex="hi" style:country-complex="IN" style:font-name-asian="Microsoft YaHei" style:font-name-complex="Arial" style:font-size-asian="10pt" style:font-size-complex="10pt" style:font-weight-asian="normal" style:font-weight-complex="normal" style:font-style-asian="normal" style:font-style-complex="normal" style:text-emphasize="none" style:font-relief="none" style:text-overline-style="none" style:text-overline-color="font-color"/>
+    </style:style>
+    <style:style style:name="T2" style:family="text">
+      <style:text-properties fo:color="#c9211e"/>
+    </style:style>
+    <style:style style:name="T3" style:family="text">
+      <style:text-properties style:font-name="Liberation Sans" fo:font-size="10pt" fo:font-weight="normal" style:text-underline-style="none" style:text-underline-color="font-color" style:text-line-through-type="none" fo:font-style="normal" style:text-outline="false" fo:text-shadow="none" style:text-line-through-mode="continuous" fo:language="fr" fo:country="FR" style:language-asian="zh" style:country-asian="CN" style:language-complex="hi" style:country-complex="IN" style:font-name-asian="Microsoft YaHei" style:font-name-complex="Arial" style:font-size-asian="10pt" style:font-size-complex="10pt" style:font-weight-asian="normal" style:font-weight-complex="normal" style:font-style-asian="normal" style:font-style-complex="normal" style:text-emphasize="none" style:font-relief="none" style:text-overline-style="none" style:text-overline-color="font-color" fo:color="#ff0000"/>
     </style:style>
   </office:automatic-styles>
   <office:body>
@@ -79,18 +92,22 @@
         <table:table-column table:style-name="co1" table:default-cell-style-name="ce2"/>
         <table:table-column table:style-name="co2" table:default-cell-style-name="Default"/>
         <table:table-column table:style-name="co3" table:default-cell-style-name="ce4"/>
-        <table:table-column table:style-name="co4" table:number-columns-repeated="1021" table:default-cell-style-name="Default"/>
+        <table:table-column table:style-name="co4" table:default-cell-style-name="ce2"/>
+        <table:table-column table:style-name="co5" table:number-columns-repeated="1020" table:default-cell-style-name="Default"/>
         <table:table-row table:style-name="ro1">
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>test_name</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>parameters summary</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
+            <text:p>reading speed</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>comment</text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="1021"/>
+          <table:table-cell table:number-columns-repeated="1020"/>
         </table:table-row>
         <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -134,7 +151,10 @@
             <text:p>Continuous ram1 check</text:p>
             <text:p>Continuous ram2 check</text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="1021"/>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Nominal case</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="1020"/>
         </table:table-row>
         <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -178,7 +198,10 @@
             <text:p>Continuous ram1 check</text:p>
             <text:p>Continuous ram2 check</text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="1021"/>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Low limit case</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="1020"/>
         </table:table-row>
         <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -222,13 +245,17 @@
             <text:p>Continuous ram1 check</text:p>
             <text:p>Continuous ram2 check</text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="1021"/>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>High limite case</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="1020"/>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell table:style-name="ce7"/>
           <table:table-cell table:style-name="ce9"/>
           <table:table-cell table:style-name="ce11"/>
-          <table:table-cell table:style-name="ce9" table:number-columns-repeated="1021"/>
+          <table:table-cell table:style-name="ce7"/>
+          <table:table-cell table:style-name="ce9" table:number-columns-repeated="1020"/>
         </table:table-row>
         <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -272,22 +299,503 @@
             <text:p>Continuous ram1 check</text:p>
             <text:p>Continuous ram2 check</text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="1021"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1" table:number-rows-repeated="7">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Short simulation</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="1020"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro4">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>tb_mux_squid_top_test_variant_debug01.json</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce3" office:value-type="string" calcext:value-type="string">
+            <text:p>« inter_squid_gain »: 255,</text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_sample_by_pixel": 8,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_pixel_by_frame": 2,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_frame_by_pulse": 3,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_pulse": 2,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"mux_squid"/ « mode »: 0,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"mux_squid"/ «min_value »: 1,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"mux_squid"/ « max_value »: 10,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">« pixel_result »/ « mode »: 1,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">« pixel_result »/ « min_value »: 10,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">« pixel_result »/ « max_value »: 20</text:span>
+            </text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Continuous data valid</text:p>
+            <text:p>
+              <text:span text:style-name="T2">sporadic ram1 check</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T2">sporadic ram2 check</text:span>
+            </text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Sporadic RAM writting</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="1020"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro4">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>tb_mux_squid_top_test_variant_debug02.json</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce3" office:value-type="string" calcext:value-type="string">
+            <text:p>
+              <text:span text:style-name="T2">« inter_squid_gain »: 0,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_sample_by_pixel": 8,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_pixel_by_frame": 34,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_frame_by_pulse": 2048,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_pulse": 1,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"mux_squid"/ « mode »: 1,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"mux_squid"/ «min_value »:- 8192,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"mux_squid"/ « max_value »: 8191,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">« pixel_result »/ « mode »: 1,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">« pixel_result »/ « min_value »: 0,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">« pixel_result »/ « max_value »: 65535</text:span>
+            </text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Continuous data valid</text:p>
+            <text:p>Continuous ram1 check</text:p>
+            <text:p>Continuous ram2 check</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="8">
+            <text:p>inter_squid_gain variation by step of 32</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="1020"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro4">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>tb_mux_squid_top_test_variant_debug03.json</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce3" office:value-type="string" calcext:value-type="string">
+            <text:p>
+              <text:span text:style-name="T2">« inter_squid_gain »: 31,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_sample_by_pixel": 8,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_pixel_by_frame": 34,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_frame_by_pulse": 2048,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_pulse": 1,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"mux_squid"/ « mode »: 1,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"mux_squid"/ «min_value »:- 8192,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"mux_squid"/ « max_value »: 8191,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">« pixel_result »/ « mode »: 1,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">« pixel_result »/ « min_value »: 0,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">« pixel_result »/ « max_value »: 65535</text:span>
+            </text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Continuous data valid</text:p>
+            <text:p>Continuous ram1 check</text:p>
+            <text:p>Continuous ram2 check</text:p>
+          </table:table-cell>
+          <table:covered-table-cell/>
+          <table:table-cell table:number-columns-repeated="1020"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro4">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>tb_mux_squid_top_test_variant_debug04.json</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce3" office:value-type="string" calcext:value-type="string">
+            <text:p>
+              <text:span text:style-name="T2">« inter_squid_gain »: 63,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_sample_by_pixel": 8,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_pixel_by_frame": 34,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_frame_by_pulse": 2048,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_pulse": 1,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"mux_squid"/ « mode »: 1,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"mux_squid"/ «min_value »:- 8192,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"mux_squid"/ « max_value »: 8191,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">« pixel_result »/ « mode »: 1,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">« pixel_result »/ « min_value »: 0,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">« pixel_result »/ « max_value »: 65535</text:span>
+            </text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Continuous data valid</text:p>
+            <text:p>Continuous ram1 check</text:p>
+            <text:p>Continuous ram2 check</text:p>
+          </table:table-cell>
+          <table:covered-table-cell/>
+          <table:table-cell table:number-columns-repeated="1020"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro4">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>tb_mux_squid_top_test_variant_debug05.json</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce3" office:value-type="string" calcext:value-type="string">
+            <text:p>
+              <text:span text:style-name="T2">« inter_squid_gain »: 95,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_sample_by_pixel": 8,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_pixel_by_frame": 34,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_frame_by_pulse": 2048,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_pulse": 1,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"mux_squid"/ « mode »: 1,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"mux_squid"/ «min_value »:- 8192,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"mux_squid"/ « max_value »: 8191,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">« pixel_result »/ « mode »: 1,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">« pixel_result »/ « min_value »: 0,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">« pixel_result »/ « max_value »: 65535</text:span>
+            </text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Continuous data valid</text:p>
+            <text:p>Continuous ram1 check</text:p>
+            <text:p>Continuous ram2 check</text:p>
+          </table:table-cell>
+          <table:covered-table-cell/>
+          <table:table-cell table:number-columns-repeated="1020"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro4">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>tb_mux_squid_top_test_variant_debug06.json</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce3" office:value-type="string" calcext:value-type="string">
+            <text:p>
+              <text:span text:style-name="T2">« inter_squid_gain »: 127,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_sample_by_pixel": 8,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_pixel_by_frame": 34,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_frame_by_pulse": 2048,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_pulse": 1,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"mux_squid"/ « mode »: 1,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"mux_squid"/ «min_value »:- 8192,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"mux_squid"/ « max_value »: 8191,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">« pixel_result »/ « mode »: 1,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">« pixel_result »/ « min_value »: 0,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">« pixel_result »/ « max_value »: 65535</text:span>
+            </text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Continuous data valid</text:p>
+            <text:p>Continuous ram1 check</text:p>
+            <text:p>Continuous ram2 check</text:p>
+          </table:table-cell>
+          <table:covered-table-cell/>
+          <table:table-cell table:number-columns-repeated="1020"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro4">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>tb_mux_squid_top_test_variant_debug07.json</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce3" office:value-type="string" calcext:value-type="string">
+            <text:p>
+              <text:span text:style-name="T2">« inter_squid_gain »: 159,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_sample_by_pixel": 8,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_pixel_by_frame": 34,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_frame_by_pulse": 2048,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_pulse": 1,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"mux_squid"/ « mode »: 1,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"mux_squid"/ «min_value »:- 8192,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"mux_squid"/ « max_value »: 8191,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">« pixel_result »/ « mode »: 1,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">« pixel_result »/ « min_value »: 0,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">« pixel_result »/ « max_value »: 65535</text:span>
+            </text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Continuous data valid</text:p>
+            <text:p>Continuous ram1 check</text:p>
+            <text:p>Continuous ram2 check</text:p>
+          </table:table-cell>
+          <table:covered-table-cell/>
+          <table:table-cell table:number-columns-repeated="1020"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro4">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>tb_mux_squid_top_test_variant_debug08.json</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce3" office:value-type="string" calcext:value-type="string">
+            <text:p>
+              <text:span text:style-name="T2">« inter_squid_gain »: 191,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_sample_by_pixel": 8,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_pixel_by_frame": 34,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_frame_by_pulse": 2048,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_pulse": 1,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"mux_squid"/ « mode »: 1,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"mux_squid"/ «min_value »:- 8192,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"mux_squid"/ « max_value »: 8191,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">« pixel_result »/ « mode »: 1,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">« pixel_result »/ « min_value »: 0,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">« pixel_result »/ « max_value »: 65535</text:span>
+            </text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Continuous data valid</text:p>
+            <text:p>Continuous ram1 check</text:p>
+            <text:p>Continuous ram2 check</text:p>
+          </table:table-cell>
+          <table:covered-table-cell/>
+          <table:table-cell table:number-columns-repeated="1020"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro4">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>tb_mux_squid_top_test_variant_debug09.json</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce3" office:value-type="string" calcext:value-type="string">
+            <text:p>
+              <text:span text:style-name="T2">« inter_squid_gain »: 223,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_sample_by_pixel": 8,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_pixel_by_frame": 34,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_frame_by_pulse": 2048,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_pulse": 1,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"mux_squid"/ « mode »: 1,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"mux_squid"/ «min_value »:- 8192,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"mux_squid"/ « max_value »: 8191,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">« pixel_result »/ « mode »: 1,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">« pixel_result »/ « min_value »: 0,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">« pixel_result »/ « max_value »: 65535</text:span>
+            </text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Continuous data valid</text:p>
+            <text:p>Continuous ram1 check</text:p>
+            <text:p>Continuous ram2 check</text:p>
+          </table:table-cell>
+          <table:covered-table-cell/>
+          <table:table-cell table:number-columns-repeated="1020"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro4">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>tb_mux_squid_top_test_variant_debug10.json</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce3" office:value-type="string" calcext:value-type="string">
+            <text:p>« inter_squid_gain »: 255,</text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_sample_by_pixel": 8,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_pixel_by_frame": 34,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_frame_by_pulse": 2048,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_pulse": 1,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"mux_squid"/ « mode »: 1,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"mux_squid"/ «min_value »:- 8192,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"mux_squid"/ « max_value »: 8191,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">« pixel_result »/ « mode »: 1,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">« pixel_result »/ « min_value »: 0,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">« pixel_result »/ « max_value »: 65535</text:span>
+            </text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>
+              <text:span text:style-name="T3">sporadic data valid</text:span>
+            </text:p>
+            <text:p>Continuous ram1 check</text:p>
+            <text:p>Continuous ram2 check</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Sporadic data input stream test (non nominal case)</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="1020"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
           <table:table-cell table:number-columns-repeated="1024"/>
         </table:table-row>
-        <table:table-row table:style-name="ro1" table:number-rows-repeated="2">
+        <table:table-row table:style-name="ro1" table:number-rows-repeated="13">
           <table:table-cell table:style-name="Default"/>
           <table:table-cell/>
           <table:table-cell table:style-name="Default"/>
           <table:table-cell table:number-columns-repeated="1021"/>
         </table:table-row>
         <table:table-row table:style-name="ro1">
-          <table:table-cell table:number-columns-repeated="1024"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell table:number-columns-repeated="1024"/>
+          <table:table-cell table:style-name="Default"/>
+          <table:table-cell/>
+          <table:table-cell table:style-name="Default"/>
+          <table:table-cell table:number-columns-repeated="1021"/>
         </table:table-row>
       </table:table>
       <table:named-expressions/>
@@ -299,11 +807,11 @@
 <file path=meta.xml><?xml version="1.0" encoding="utf-8"?>
 <office:document-meta xmlns:grddl="http://www.w3.org/2003/g/data-view#" xmlns:meta="urn:oasis:names:tc:opendocument:xmlns:meta:1.0" xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" xmlns:ooo="http://openoffice.org/2004/office" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:dc="http://purl.org/dc/elements/1.1/" office:version="1.3">
   <office:meta>
-    <dc:date>2023-05-30T13:48:22.052000000</dc:date>
-    <meta:editing-duration>PT4H41M38S</meta:editing-duration>
-    <meta:editing-cycles>13</meta:editing-cycles>
+    <dc:date>2023-06-02T11:19:28.161000000</dc:date>
+    <meta:editing-duration>PT4H54M40S</meta:editing-duration>
+    <meta:editing-cycles>15</meta:editing-cycles>
     <meta:generator>LibreOffice/7.2.4.1$Windows_X86_64 LibreOffice_project/27d75539669ac387bb498e35313b970b7fe9c4f9</meta:generator>
-    <meta:document-statistic meta:table-count="1" meta:cell-count="15" meta:object-count="0"/>
+    <meta:document-statistic meta:table-count="1" meta:cell-count="53" meta:object-count="0"/>
   </office:meta>
 </office:document-meta>
 </file>
@@ -314,15 +822,15 @@
     <config:config-item-set config:name="ooo:view-settings">
       <config:config-item config:name="VisibleAreaTop" config:type="int">0</config:config-item>
       <config:config-item config:name="VisibleAreaLeft" config:type="int">0</config:config-item>
-      <config:config-item config:name="VisibleAreaWidth" config:type="int">24533</config:config-item>
-      <config:config-item config:name="VisibleAreaHeight" config:type="int">22406</config:config-item>
+      <config:config-item config:name="VisibleAreaWidth" config:type="int">33628</config:config-item>
+      <config:config-item config:name="VisibleAreaHeight" config:type="int">66362</config:config-item>
       <config:config-item-map-indexed config:name="Views">
         <config:config-item-map-entry>
           <config:config-item config:name="ViewId" config:type="string">view1</config:config-item>
           <config:config-item-map-named config:name="Tables">
             <config:config-item-map-entry config:name="Feuille1">
-              <config:config-item config:name="CursorPositionX" config:type="int">0</config:config-item>
-              <config:config-item config:name="CursorPositionY" config:type="int">4</config:config-item>
+              <config:config-item config:name="CursorPositionX" config:type="int">5</config:config-item>
+              <config:config-item config:name="CursorPositionY" config:type="int">6</config:config-item>
               <config:config-item config:name="HorizontalSplitMode" config:type="short">0</config:config-item>
               <config:config-item config:name="VerticalSplitMode" config:type="short">0</config:config-item>
               <config:config-item config:name="HorizontalSplitPosition" config:type="int">0</config:config-item>
@@ -331,7 +839,7 @@
               <config:config-item config:name="PositionLeft" config:type="int">0</config:config-item>
               <config:config-item config:name="PositionRight" config:type="int">0</config:config-item>
               <config:config-item config:name="PositionTop" config:type="int">0</config:config-item>
-              <config:config-item config:name="PositionBottom" config:type="int">0</config:config-item>
+              <config:config-item config:name="PositionBottom" config:type="int">3</config:config-item>
               <config:config-item config:name="ZoomType" config:type="short">0</config:config-item>
               <config:config-item config:name="ZoomValue" config:type="int">100</config:config-item>
               <config:config-item config:name="PageViewZoomValue" config:type="int">60</config:config-item>
@@ -543,9 +1051,9 @@
         </style:region-left>
         <style:region-right>
           <text:p>
-            <text:date style:data-style-name="N2" text:date-value="2023-05-30">00/00/0000</text:date>
+            <text:date style:data-style-name="N2" text:date-value="2023-06-02">00/00/0000</text:date>
             , 
-            <text:time style:data-style-name="N2" text:time-value="10:51:11.226000000">00:00:00</text:time>
+            <text:time style:data-style-name="N2" text:time-value="09:30:58.442000000">00:00:00</text:time>
           </text:p>
         </style:region-right>
       </style:header>

</xml_diff>

<commit_message>
ci,mux_squid: add the tb_mux_squid_top_test_variant_debug11.json test: disable the adc input and increment the second input in order to output the memory content.
</commit_message>
<xml_diff>
--- a/simu/conf/fpasim/mux_squid/mux_squid_top_test_list.xlsx
+++ b/simu/conf/fpasim/mux_squid/mux_squid_top_test_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fpasim-fw-hardware\simu\conf\fpasim\mux_squid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14DB1F7C-B041-4D56-976A-1A7CD12E8D72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18AF7E7D-F4C0-4370-A110-EC29B6C5540F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="46">
   <si>
     <t>test_name</t>
   </si>
@@ -1005,6 +1005,92 @@
 « pixel_result »/ « min_value »: 0,
 « pixel_result »/ « max_value »: 65535</t>
     </r>
+  </si>
+  <si>
+    <t>tb_mux_squid_top_test_variant_debug11.json</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">« inter_squid_gain »: 255,
+"nb_sample_by_pixel": </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>8</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">,
+"nb_pixel_by_frame": </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,
+"nb_frame_by_pulse": 2048,
+"nb_pulse": 8,
+"mux_squid"/ « mode »: 0,
+"mux_squid"/ «min_value »:0,
+"mux_squid"/ « max_value »: 0,
+« pixel_result »/ « mode »: 0,
+« pixel_result »/ « min_value »: 0,
+« pixel_result »/ « max_value »: 65535</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Liberation Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">continuous data valid
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Continuous ram1 check
+Continuous ram2 check</t>
+    </r>
+  </si>
+  <si>
+    <t>Auto-check
+ disable adc data (=0) =&gt; output the memory content (non nominal case)
+1 pixels by frame</t>
   </si>
 </sst>
 </file>
@@ -1099,17 +1185,17 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1393,8 +1479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8:D15"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1429,7 +1515,7 @@
       <c r="C2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="8" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1443,7 +1529,7 @@
       <c r="C3" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="8" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1457,7 +1543,7 @@
       <c r="C4" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="8" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1477,7 +1563,7 @@
       <c r="C6" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="8" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1491,7 +1577,7 @@
       <c r="C7" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="8" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1505,7 +1591,7 @@
       <c r="C8" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="11" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1519,7 +1605,7 @@
       <c r="C9" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="8"/>
+      <c r="D9" s="12"/>
     </row>
     <row r="10" spans="1:4" ht="162.75" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
@@ -1531,7 +1617,7 @@
       <c r="C10" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="8"/>
+      <c r="D10" s="12"/>
     </row>
     <row r="11" spans="1:4" ht="162.75" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
@@ -1543,7 +1629,7 @@
       <c r="C11" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="8"/>
+      <c r="D11" s="12"/>
     </row>
     <row r="12" spans="1:4" ht="162.75" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
@@ -1555,7 +1641,7 @@
       <c r="C12" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="8"/>
+      <c r="D12" s="12"/>
     </row>
     <row r="13" spans="1:4" ht="162.75" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
@@ -1567,7 +1653,7 @@
       <c r="C13" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="8"/>
+      <c r="D13" s="12"/>
     </row>
     <row r="14" spans="1:4" ht="162.75" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
@@ -1579,7 +1665,7 @@
       <c r="C14" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="8"/>
+      <c r="D14" s="12"/>
     </row>
     <row r="15" spans="1:4" ht="162.75" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
@@ -1591,7 +1677,7 @@
       <c r="C15" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="8"/>
+      <c r="D15" s="12"/>
     </row>
     <row r="16" spans="1:4" ht="165" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
@@ -1603,13 +1689,27 @@
       <c r="C16" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="D16" s="8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="11"/>
-      <c r="B19" s="12" t="s">
+    <row r="17" spans="1:4" ht="165" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="9"/>
+      <c r="B19" s="10" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>